<commit_message>
Notes from Ann Arbor, load directory template
</commit_message>
<xml_diff>
--- a/AnnArbor2012/ActivityFeedOptionComparisons.xlsx
+++ b/AnnArbor2012/ActivityFeedOptionComparisons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="21460" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15520" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RDBMSStorage" sheetId="2" r:id="rId1"/>
@@ -210,12 +210,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -903,9 +897,9 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1225,10 +1219,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1548,10 +1540,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1888,7 +1878,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1945,50 +1935,50 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>20000</v>
       </c>
       <c r="C3">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3">
-        <v>61091</v>
-      </c>
-      <c r="H3" s="1"/>
+        <v>60683</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>20000</v>
       </c>
       <c r="C4">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
       <c r="G4">
-        <v>60683</v>
-      </c>
+        <v>61091</v>
+      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
@@ -2040,83 +2030,83 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>20000</v>
       </c>
       <c r="C7">
-        <v>375</v>
+        <v>442</v>
       </c>
       <c r="D7">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="E7">
-        <v>380</v>
+        <v>412</v>
       </c>
       <c r="F7">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>64323</v>
+        <v>63246</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>20000</v>
       </c>
       <c r="C8">
-        <v>442</v>
+        <v>499</v>
       </c>
       <c r="D8">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E8">
-        <v>412</v>
+        <v>480</v>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>63246</v>
+        <v>64053</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>20000</v>
       </c>
       <c r="C9">
-        <v>499</v>
+        <v>375</v>
       </c>
       <c r="D9">
-        <v>96</v>
+        <v>153</v>
       </c>
       <c r="E9">
-        <v>480</v>
+        <v>380</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>64053</v>
+        <v>64323</v>
       </c>
       <c r="H9" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD9">
-    <sortCondition ref="E3:E9"/>
+    <sortCondition ref="D3:D9"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
cfg file for postgres operation
</commit_message>
<xml_diff>
--- a/AnnArbor2012/ActivityFeedOptionComparisons.xlsx
+++ b/AnnArbor2012/ActivityFeedOptionComparisons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15520" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15520" tabRatio="589" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RDBMSStorage" sheetId="2" r:id="rId1"/>
@@ -12,11 +12,15 @@
     <sheet name="SeparateRun1" sheetId="4" r:id="rId3"/>
     <sheet name="SeparateRun2" sheetId="5" r:id="rId4"/>
     <sheet name="Summary" sheetId="3" r:id="rId5"/>
+    <sheet name="Vanilla 1.4.0" sheetId="7" r:id="rId6"/>
+    <sheet name="JPAStorage" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="aggregate" localSheetId="6">JPAStorage!$A$1:$J$9</definedName>
     <definedName name="aggregate" localSheetId="3">SeparateRun2!$A$1:$J$9</definedName>
     <definedName name="aggregate" localSheetId="1">VanillaNakamura!$A$1:$J$9</definedName>
     <definedName name="aggregate_1" localSheetId="0">RDBMSStorage!$A$1:$J$9</definedName>
+    <definedName name="aggregate_1" localSheetId="5">'Vanilla 1.4.0'!$A$1:$J$9</definedName>
     <definedName name="aggregate_multiple_connections_separate_activity_tables" localSheetId="2">SeparateRun1!$A$1:$J$9</definedName>
   </definedNames>
   <calcPr calcId="130407" concurrentCalc="0"/>
@@ -94,11 +98,43 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="5" name="Connection5" type="6" refreshedVersion="0">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:chris:oae-installations:sparse-181:vanillaNakamura1.4.0:run1:results:aggregate.csv" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="Connection6" type="6" refreshedVersion="0">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:chris:oae-installations:sparse-181:jpaActivityStorage:run1:results:aggregate.csv" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="35">
   <si>
     <t>sampler_label</t>
   </si>
@@ -203,6 +239,22 @@
   </si>
   <si>
     <t>Separate Run 2 - search feed failure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vanilla 1.4.0 - search success</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vanilla 1.4.0 - search fail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPA Based - search success</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPA Based - search fail</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -210,6 +262,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -266,6 +324,14 @@
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="aggregate" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="aggregate_1" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="aggregate" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1540,6 +1606,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1861,7 +1928,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1875,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1886,7 +1952,7 @@
     <col min="1" max="1" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1909,7 +1975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1933,7 +1999,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1956,7 +2022,7 @@
         <v>60683</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1980,7 +2046,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2004,7 +2070,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2028,7 +2094,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2052,7 +2118,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2076,7 +2142,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2100,8 +2166,135 @@
       </c>
       <c r="H9" s="1"/>
     </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>3383</v>
+      </c>
+      <c r="C10">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>32</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>60105</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>8.2810717660248407</v>
+      </c>
+      <c r="J10">
+        <v>92.691016238874496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>3378</v>
+      </c>
+      <c r="C11">
+        <v>199</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>60142</v>
+      </c>
+      <c r="H11">
+        <v>1.18413262285375E-3</v>
+      </c>
+      <c r="I11">
+        <v>8.2849553745520907</v>
+      </c>
+      <c r="J11">
+        <v>92.802890514057196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>1895</v>
+      </c>
+      <c r="C12">
+        <v>1837</v>
+      </c>
+      <c r="D12">
+        <v>364</v>
+      </c>
+      <c r="E12">
+        <v>3541</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>70044</v>
+      </c>
+      <c r="H12">
+        <v>3.6939313984168799E-3</v>
+      </c>
+      <c r="I12">
+        <v>2.2658167761313202</v>
+      </c>
+      <c r="J12">
+        <v>35.049928911119601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>1889</v>
+      </c>
+      <c r="C13">
+        <v>889</v>
+      </c>
+      <c r="D13">
+        <v>32</v>
+      </c>
+      <c r="E13">
+        <v>781</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>64345</v>
+      </c>
+      <c r="H13">
+        <v>1.58814187400741E-3</v>
+      </c>
+      <c r="I13">
+        <v>2.2606293860278899</v>
+      </c>
+      <c r="J13">
+        <v>8.4019098967458405E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD9">
     <sortCondition ref="D3:D9"/>
   </sortState>
@@ -2113,4 +2306,649 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A8" activeCellId="1" sqref="A6:XFD6 A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>3394</v>
+      </c>
+      <c r="C2">
+        <v>164</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>60059</v>
+      </c>
+      <c r="H2" s="1">
+        <v>8.8391278727165503E-4</v>
+      </c>
+      <c r="I2">
+        <v>8.2963412010872695</v>
+      </c>
+      <c r="J2">
+        <v>1.1565611280726199E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>3390</v>
+      </c>
+      <c r="C3">
+        <v>347</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>199649</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5.8997050147492603E-4</v>
+      </c>
+      <c r="I3">
+        <v>8.2878398564419005</v>
+      </c>
+      <c r="J3">
+        <v>3.03914201299161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>3386</v>
+      </c>
+      <c r="C4">
+        <v>177</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>60085</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5.9066745422327197E-4</v>
+      </c>
+      <c r="I4">
+        <v>8.2800850016995398</v>
+      </c>
+      <c r="J4">
+        <v>11.175465422361301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>3383</v>
+      </c>
+      <c r="C5">
+        <v>159</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>44</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>60097</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>8.2774853865558704</v>
+      </c>
+      <c r="J5">
+        <v>0.39328301512849301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>3383</v>
+      </c>
+      <c r="C6">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>60105</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>8.2810717660248407</v>
+      </c>
+      <c r="J6">
+        <v>92.691016238874496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>3380</v>
+      </c>
+      <c r="C7">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>60072</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2.9585798816567999E-4</v>
+      </c>
+      <c r="I7">
+        <v>8.2816140816841504</v>
+      </c>
+      <c r="J7">
+        <v>18.310956634387502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>3378</v>
+      </c>
+      <c r="C8">
+        <v>199</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>60142</v>
+      </c>
+      <c r="H8">
+        <v>1.18413262285375E-3</v>
+      </c>
+      <c r="I8">
+        <v>8.2849553745520907</v>
+      </c>
+      <c r="J8">
+        <v>92.802890514057196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>23694</v>
+      </c>
+      <c r="C9">
+        <v>170</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>199649</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5.0645733096986499E-4</v>
+      </c>
+      <c r="I9">
+        <v>57.910726462616097</v>
+      </c>
+      <c r="J9">
+        <v>217.90813799807799</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A8" activeCellId="1" sqref="A6:XFD6 A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1907</v>
+      </c>
+      <c r="C2">
+        <v>562</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>756</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>61654</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5.2438384897745096E-4</v>
+      </c>
+      <c r="I2">
+        <v>2.2769741437466702</v>
+      </c>
+      <c r="J2">
+        <v>1.8831285857566699E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1906</v>
+      </c>
+      <c r="C3">
+        <v>1227</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+      <c r="E3">
+        <v>1685</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>63940</v>
+      </c>
+      <c r="H3">
+        <v>2.6232948583420701E-3</v>
+      </c>
+      <c r="I3">
+        <v>2.2763454742406299</v>
+      </c>
+      <c r="J3">
+        <v>0.84152671712705096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1902</v>
+      </c>
+      <c r="C4">
+        <v>1020</v>
+      </c>
+      <c r="D4">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <v>950</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>64363</v>
+      </c>
+      <c r="H4">
+        <v>2.6288117770767601E-3</v>
+      </c>
+      <c r="I4">
+        <v>2.2720702597709699</v>
+      </c>
+      <c r="J4">
+        <v>3.0678900353682002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1899</v>
+      </c>
+      <c r="C5">
+        <v>1448</v>
+      </c>
+      <c r="D5">
+        <v>119</v>
+      </c>
+      <c r="E5">
+        <v>1769</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>65080</v>
+      </c>
+      <c r="H5">
+        <v>3.1595576619273301E-3</v>
+      </c>
+      <c r="I5">
+        <v>2.26871962496236</v>
+      </c>
+      <c r="J5">
+        <v>0.12118654394793001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1895</v>
+      </c>
+      <c r="C6">
+        <v>1837</v>
+      </c>
+      <c r="D6">
+        <v>364</v>
+      </c>
+      <c r="E6">
+        <v>3541</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>70044</v>
+      </c>
+      <c r="H6">
+        <v>3.6939313984168799E-3</v>
+      </c>
+      <c r="I6">
+        <v>2.2658167761313202</v>
+      </c>
+      <c r="J6">
+        <v>35.049928911119601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1889</v>
+      </c>
+      <c r="C7">
+        <v>605</v>
+      </c>
+      <c r="D7">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>781</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>61645</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5.2938062466913703E-4</v>
+      </c>
+      <c r="I7">
+        <v>2.2605617537842502</v>
+      </c>
+      <c r="J7">
+        <v>1.73937073564291</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1889</v>
+      </c>
+      <c r="C8">
+        <v>889</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>781</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>64345</v>
+      </c>
+      <c r="H8">
+        <v>1.58814187400741E-3</v>
+      </c>
+      <c r="I8">
+        <v>2.2606293860278899</v>
+      </c>
+      <c r="J8">
+        <v>8.4019098967458405E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>13287</v>
+      </c>
+      <c r="C9">
+        <v>1084</v>
+      </c>
+      <c r="D9">
+        <v>92</v>
+      </c>
+      <c r="E9">
+        <v>1595</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>70044</v>
+      </c>
+      <c r="H9">
+        <v>2.1073229472416601E-3</v>
+      </c>
+      <c r="I9">
+        <v>15.8647904813645</v>
+      </c>
+      <c r="J9">
+        <v>40.850939283550098</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>